<commit_message>
add full denormalization results
</commit_message>
<xml_diff>
--- a/results/statistics/summary.xlsx
+++ b/results/statistics/summary.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="~3e5" sheetId="1" r:id="rId1"/>
-    <sheet name="~5e7" sheetId="4" r:id="rId2"/>
+    <sheet name="~3e6" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -159,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -184,6 +184,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -202,14 +210,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,7 +513,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -519,69 +525,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="18" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19">
+      <c r="D4" s="20"/>
+      <c r="E4" s="12">
         <v>10000</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19">
+      <c r="D5" s="20"/>
+      <c r="E5" s="12">
         <v>50000</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19">
+      <c r="D6" s="20"/>
+      <c r="E6" s="12">
         <v>6850</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19">
+      <c r="D7" s="20"/>
+      <c r="E7" s="12">
         <v>396892</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19">
+      <c r="D8" s="20"/>
+      <c r="E8" s="12">
         <v>396892</v>
       </c>
     </row>
@@ -589,20 +595,20 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="12" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="13"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
@@ -678,7 +684,7 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -703,7 +709,7 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="10"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
@@ -734,10 +740,10 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="11"/>
+      <c r="B18" s="15"/>
       <c r="D18" s="6"/>
       <c r="E18" s="4">
         <f>SUM(E13:E16)</f>
@@ -761,31 +767,31 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="14" t="s">
+      <c r="E23" s="19"/>
+      <c r="F23" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="15"/>
+      <c r="G23" s="19"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
@@ -861,7 +867,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -886,7 +892,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="10"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="1" t="s">
         <v>16</v>
       </c>
@@ -917,10 +923,10 @@
       <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="11"/>
+      <c r="B30" s="15"/>
       <c r="D30" s="6"/>
       <c r="E30" s="4">
         <f>SUM(E25:E28)</f>
@@ -970,7 +976,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -982,90 +988,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="18" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19">
-        <v>10000</v>
+      <c r="D4" s="20"/>
+      <c r="E4">
+        <v>300000</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19">
-        <v>50000</v>
+      <c r="D5" s="20"/>
+      <c r="E5">
+        <v>1500000</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19">
-        <v>6850</v>
+      <c r="D6" s="20"/>
+      <c r="E6">
+        <v>205500</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19">
-        <v>396892</v>
+      <c r="D7" s="20"/>
+      <c r="E7">
+        <v>3780426</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19">
-        <v>396892</v>
+      <c r="D8" s="20"/>
+      <c r="E8">
+        <v>3780426</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="12" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="13"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
@@ -1100,19 +1106,19 @@
       <c r="C13" s="2">
         <v>13</v>
       </c>
-      <c r="D13" s="7">
-        <v>3.2</v>
+      <c r="D13" s="10">
+        <v>3.44</v>
       </c>
       <c r="E13" s="8">
         <f>D13*C25/C32</f>
-        <v>1.7333333333333334</v>
-      </c>
-      <c r="F13" s="7">
-        <v>0.63</v>
+        <v>1.8633333333333333</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.65</v>
       </c>
       <c r="G13" s="8">
         <f>F13*C25/C32</f>
-        <v>0.34125</v>
+        <v>0.35208333333333336</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1125,14 +1131,14 @@
       <c r="C14" s="2">
         <v>1</v>
       </c>
-      <c r="D14" s="7">
-        <v>2.12</v>
+      <c r="D14" s="10">
+        <v>2.2000000000000002</v>
       </c>
       <c r="E14" s="8">
         <f>D14*C26/C32</f>
-        <v>8.8333333333333333E-2</v>
-      </c>
-      <c r="F14" s="7" t="s">
+        <v>9.1666666666666674E-2</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G14" s="8" t="e">
@@ -1141,7 +1147,7 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1150,14 +1156,14 @@
       <c r="C15" s="2">
         <v>10</v>
       </c>
-      <c r="D15" s="7">
-        <v>2.12</v>
+      <c r="D15" s="10">
+        <v>1.54</v>
       </c>
       <c r="E15" s="8">
         <f>D15*C27/C32</f>
-        <v>0.88333333333333341</v>
-      </c>
-      <c r="F15" s="7" t="s">
+        <v>0.64166666666666672</v>
+      </c>
+      <c r="F15" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="8" t="e">
@@ -1166,21 +1172,21 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="10"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="2">
         <v>10</v>
       </c>
-      <c r="D16" s="7">
-        <v>2.29</v>
+      <c r="D16" s="10">
+        <v>2.38</v>
       </c>
       <c r="E16" s="8">
         <f>D16*C28/C32</f>
-        <v>0.95416666666666661</v>
-      </c>
-      <c r="F16" s="7" t="s">
+        <v>0.99166666666666659</v>
+      </c>
+      <c r="F16" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G16" s="8" t="e">
@@ -1197,14 +1203,14 @@
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="11"/>
+      <c r="B18" s="15"/>
       <c r="D18" s="6"/>
       <c r="E18" s="8">
         <f>SUM(E13:E16)</f>
-        <v>3.6591666666666667</v>
+        <v>3.5883333333333334</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="8" t="e">
@@ -1224,31 +1230,31 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="14" t="s">
+      <c r="E23" s="19"/>
+      <c r="F23" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="15"/>
+      <c r="G23" s="19"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
@@ -1284,18 +1290,16 @@
         <v>13</v>
       </c>
       <c r="D25" s="7">
-        <v>1.35</v>
+        <v>1.33</v>
       </c>
       <c r="E25" s="8">
         <f>D25*C25/C32</f>
-        <v>0.73125000000000007</v>
-      </c>
-      <c r="F25" s="7">
-        <v>1.31</v>
-      </c>
+        <v>0.72041666666666659</v>
+      </c>
+      <c r="F25" s="7"/>
       <c r="G25" s="8">
         <f>F25*C25/C32</f>
-        <v>0.70958333333333334</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1309,22 +1313,20 @@
         <v>1</v>
       </c>
       <c r="D26" s="7">
-        <v>4.46</v>
+        <v>6.42</v>
       </c>
       <c r="E26" s="8">
         <f>D26*C26/C32</f>
-        <v>0.18583333333333332</v>
-      </c>
-      <c r="F26" s="7">
-        <v>4.46</v>
-      </c>
+        <v>0.26750000000000002</v>
+      </c>
+      <c r="F26" s="7"/>
       <c r="G26" s="8">
         <f>F26*C26/C32</f>
-        <v>0.18583333333333332</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1334,22 +1336,20 @@
         <v>10</v>
       </c>
       <c r="D27" s="7">
-        <v>1.97</v>
+        <v>1.42</v>
       </c>
       <c r="E27" s="8">
         <f>D27*C27/C32</f>
-        <v>0.8208333333333333</v>
-      </c>
-      <c r="F27" s="7">
-        <v>1.97</v>
-      </c>
+        <v>0.59166666666666667</v>
+      </c>
+      <c r="F27" s="7"/>
       <c r="G27" s="8">
         <f>F27*C27/C32</f>
-        <v>0.8208333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="10"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="2" t="s">
         <v>16</v>
       </c>
@@ -1357,18 +1357,16 @@
         <v>10</v>
       </c>
       <c r="D28" s="7">
-        <v>5.86</v>
+        <v>5.31</v>
       </c>
       <c r="E28" s="8">
         <f>D28*C28/C32</f>
-        <v>2.4416666666666669</v>
-      </c>
-      <c r="F28" s="7">
-        <v>1.85</v>
-      </c>
+        <v>2.2124999999999999</v>
+      </c>
+      <c r="F28" s="7"/>
       <c r="G28" s="8">
         <f>F28*C28/C32</f>
-        <v>0.77083333333333337</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1380,19 +1378,19 @@
       <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="11"/>
+      <c r="B30" s="15"/>
       <c r="D30" s="6"/>
       <c r="E30" s="8">
         <f>SUM(E25:E28)</f>
-        <v>4.1795833333333334</v>
+        <v>3.7920833333333333</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="8">
         <f>SUM(G25:G28)</f>
-        <v>2.4870833333333335</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1410,11 +1408,6 @@
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="D10:E11"/>
-    <mergeCell ref="F10:G11"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C3:E3"/>
@@ -1422,6 +1415,11 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="D10:E11"/>
+    <mergeCell ref="F10:G11"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add results for 10^5 and 10^6 DT table size
</commit_message>
<xml_diff>
--- a/results/statistics/summary.xlsx
+++ b/results/statistics/summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="18990" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="~3e5" sheetId="1" r:id="rId1"/>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -975,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1114,11 +1114,11 @@
         <v>1.8633333333333333</v>
       </c>
       <c r="F13" s="10">
-        <v>0.65</v>
+        <v>0.61</v>
       </c>
       <c r="G13" s="8">
         <f>F13*C25/C32</f>
-        <v>0.35208333333333336</v>
+        <v>0.33041666666666664</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1296,10 +1296,12 @@
         <f>D25*C25/C32</f>
         <v>0.72041666666666659</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7">
+        <v>1.36</v>
+      </c>
       <c r="G25" s="8">
         <f>F25*C25/C32</f>
-        <v>0</v>
+        <v>0.73666666666666669</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1319,10 +1321,12 @@
         <f>D26*C26/C32</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="7">
+        <v>5.41</v>
+      </c>
       <c r="G26" s="8">
         <f>F26*C26/C32</f>
-        <v>0</v>
+        <v>0.22541666666666668</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1342,10 +1346,12 @@
         <f>D27*C27/C32</f>
         <v>0.59166666666666667</v>
       </c>
-      <c r="F27" s="7"/>
+      <c r="F27" s="7">
+        <v>3.71</v>
+      </c>
       <c r="G27" s="8">
         <f>F27*C27/C32</f>
-        <v>0</v>
+        <v>1.5458333333333334</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1363,10 +1369,12 @@
         <f>D28*C28/C32</f>
         <v>2.2124999999999999</v>
       </c>
-      <c r="F28" s="7"/>
+      <c r="F28" s="7">
+        <v>2.35</v>
+      </c>
       <c r="G28" s="8">
         <f>F28*C28/C32</f>
-        <v>0</v>
+        <v>0.97916666666666663</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1390,7 +1398,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="8">
         <f>SUM(G25:G28)</f>
-        <v>0</v>
+        <v>3.4870833333333331</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1422,5 +1430,6 @@
     <mergeCell ref="A18:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix typo in 3e5 results
</commit_message>
<xml_diff>
--- a/results/statistics/summary.xlsx
+++ b/results/statistics/summary.xlsx
@@ -159,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,6 +189,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -512,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -525,68 +528,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="20"/>
+      <c r="D4" s="21"/>
       <c r="E4" s="12">
         <v>10000</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="20"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="12">
         <v>50000</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="12">
         <v>6850</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="21"/>
       <c r="E7" s="12">
         <v>396892</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="20"/>
+      <c r="D8" s="21"/>
       <c r="E8" s="12">
         <v>396892</v>
       </c>
@@ -595,20 +598,20 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="16" t="s">
+      <c r="E10" s="18"/>
+      <c r="F10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="17"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
@@ -684,7 +687,7 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -693,12 +696,12 @@
       <c r="C15" s="1">
         <v>10</v>
       </c>
-      <c r="D15" s="5">
-        <v>2.12</v>
+      <c r="D15" s="14">
+        <v>1.45</v>
       </c>
       <c r="E15" s="4">
         <f>D15*C27/C32</f>
-        <v>0.88333333333333341</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>7</v>
@@ -709,7 +712,7 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="14"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
@@ -740,14 +743,14 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="15"/>
+      <c r="B18" s="16"/>
       <c r="D18" s="6"/>
       <c r="E18" s="4">
         <f>SUM(E13:E16)</f>
-        <v>3.6591666666666667</v>
+        <v>3.38</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="4" t="e">
@@ -767,31 +770,31 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="18" t="s">
+      <c r="E23" s="20"/>
+      <c r="F23" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
@@ -867,7 +870,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -892,7 +895,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="14"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="1" t="s">
         <v>16</v>
       </c>
@@ -923,10 +926,10 @@
       <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="15"/>
+      <c r="B30" s="16"/>
       <c r="D30" s="6"/>
       <c r="E30" s="4">
         <f>SUM(E25:E28)</f>
@@ -975,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -988,68 +991,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="20"/>
+      <c r="D4" s="21"/>
       <c r="E4">
         <v>300000</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="20"/>
+      <c r="D5" s="21"/>
       <c r="E5">
         <v>1500000</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="21"/>
       <c r="E6">
         <v>205500</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="21"/>
       <c r="E7">
         <v>3780426</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="20"/>
+      <c r="D8" s="21"/>
       <c r="E8">
         <v>3780426</v>
       </c>
@@ -1058,20 +1061,20 @@
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="16" t="s">
+      <c r="E10" s="18"/>
+      <c r="F10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="17"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
@@ -1147,7 +1150,7 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1172,7 +1175,7 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="14"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1203,10 +1206,10 @@
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="15"/>
+      <c r="B18" s="16"/>
       <c r="D18" s="6"/>
       <c r="E18" s="8">
         <f>SUM(E13:E16)</f>
@@ -1230,31 +1233,31 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="18" t="s">
+      <c r="E23" s="20"/>
+      <c r="F23" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
@@ -1330,7 +1333,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1355,7 +1358,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="14"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="2" t="s">
         <v>16</v>
       </c>
@@ -1386,10 +1389,10 @@
       <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="15"/>
+      <c r="B30" s="16"/>
       <c r="D30" s="6"/>
       <c r="E30" s="8">
         <f>SUM(E25:E28)</f>

</xml_diff>